<commit_message>
Upload Y2_B2526_Log_History.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y2_B2526_Log_History.xlsx
+++ b/log_history/Y2_B2526_Log_History.xlsx
@@ -469,12 +469,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>User</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Type</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -509,12 +509,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>mai_tarek@med.asu.edu.eg</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Manual</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">

</xml_diff>